<commit_message>
the main functionalities separated out for packaging
</commit_message>
<xml_diff>
--- a/archive/tournoments_2024.xlsx
+++ b/archive/tournoments_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee16c21b72f3fde9/Documents/Internet/tennis-data/2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{5CCE082C-E7FE-4FB2-924E-9E04C25B1AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74E2499D-B630-4C99-8C5A-CD68DA1207F5}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{5CCE082C-E7FE-4FB2-924E-9E04C25B1AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EECBEE2-33A6-4F97-953C-701DCAB1971A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FB451EE0-1C45-4E3B-8988-DF9692D1A74B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2432" uniqueCount="211">
   <si>
     <t>ATP</t>
   </si>
@@ -634,6 +634,42 @@
   <si>
     <t>4th Round</t>
   </si>
+  <si>
+    <t>Montpellier</t>
+  </si>
+  <si>
+    <t>Open Sud de France</t>
+  </si>
+  <si>
+    <t>Indoor</t>
+  </si>
+  <si>
+    <t>Mmoh M.</t>
+  </si>
+  <si>
+    <t>Paire B.</t>
+  </si>
+  <si>
+    <t>Martinez P.</t>
+  </si>
+  <si>
+    <t>Escoffier A.</t>
+  </si>
+  <si>
+    <t>Blanchet U.</t>
+  </si>
+  <si>
+    <t>Mayot H.</t>
+  </si>
+  <si>
+    <t>Pouille L.</t>
+  </si>
+  <si>
+    <t>Llamas Ruiz P.</t>
+  </si>
+  <si>
+    <t>Svrcina D.</t>
+  </si>
 </sst>
 </file>
 
@@ -677,11 +713,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,9 +741,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -744,7 +781,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -850,7 +887,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -992,7 +1029,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1000,13 +1037,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155D0E9E-0A55-4076-9395-03276EB23156}">
-  <dimension ref="A1:AJ240"/>
+  <dimension ref="A1:AJ267"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D206" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D233" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A240" sqref="A240"/>
+      <selection pane="bottomRight" activeCell="A267" sqref="A267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -27013,6 +27050,2556 @@
         <v>3.29</v>
       </c>
     </row>
+    <row r="241" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>6</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C241" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D241" s="2">
+        <v>45320</v>
+      </c>
+      <c r="E241" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F241" t="s">
+        <v>201</v>
+      </c>
+      <c r="G241" t="s">
+        <v>40</v>
+      </c>
+      <c r="H241" t="s">
+        <v>41</v>
+      </c>
+      <c r="I241">
+        <v>3</v>
+      </c>
+      <c r="J241" t="s">
+        <v>202</v>
+      </c>
+      <c r="K241" t="s">
+        <v>88</v>
+      </c>
+      <c r="L241">
+        <v>133</v>
+      </c>
+      <c r="M241">
+        <v>126</v>
+      </c>
+      <c r="N241">
+        <v>497</v>
+      </c>
+      <c r="O241">
+        <v>508</v>
+      </c>
+      <c r="P241">
+        <v>6</v>
+      </c>
+      <c r="Q241">
+        <v>3</v>
+      </c>
+      <c r="R241">
+        <v>7</v>
+      </c>
+      <c r="S241">
+        <v>5</v>
+      </c>
+      <c r="Z241">
+        <v>2</v>
+      </c>
+      <c r="AA241">
+        <v>0</v>
+      </c>
+      <c r="AB241" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC241">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AD241">
+        <v>1.62</v>
+      </c>
+      <c r="AE241">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AF241">
+        <v>1.74</v>
+      </c>
+      <c r="AG241">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="AH241">
+        <v>1.74</v>
+      </c>
+      <c r="AI241">
+        <v>2.19</v>
+      </c>
+      <c r="AJ241">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="242" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>6</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D242" s="2">
+        <v>45320</v>
+      </c>
+      <c r="E242" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F242" t="s">
+        <v>201</v>
+      </c>
+      <c r="G242" t="s">
+        <v>40</v>
+      </c>
+      <c r="H242" t="s">
+        <v>41</v>
+      </c>
+      <c r="I242">
+        <v>3</v>
+      </c>
+      <c r="J242" t="s">
+        <v>203</v>
+      </c>
+      <c r="K242" t="s">
+        <v>52</v>
+      </c>
+      <c r="L242">
+        <v>112</v>
+      </c>
+      <c r="M242">
+        <v>49</v>
+      </c>
+      <c r="N242">
+        <v>551</v>
+      </c>
+      <c r="O242">
+        <v>970</v>
+      </c>
+      <c r="P242">
+        <v>2</v>
+      </c>
+      <c r="Q242">
+        <v>6</v>
+      </c>
+      <c r="R242">
+        <v>7</v>
+      </c>
+      <c r="S242">
+        <v>6</v>
+      </c>
+      <c r="T242">
+        <v>6</v>
+      </c>
+      <c r="U242">
+        <v>3</v>
+      </c>
+      <c r="Z242">
+        <v>2</v>
+      </c>
+      <c r="AA242">
+        <v>1</v>
+      </c>
+      <c r="AB242" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC242">
+        <v>3.75</v>
+      </c>
+      <c r="AD242">
+        <v>1.29</v>
+      </c>
+      <c r="AE242">
+        <v>3.05</v>
+      </c>
+      <c r="AF242">
+        <v>1.43</v>
+      </c>
+      <c r="AG242">
+        <v>3.8</v>
+      </c>
+      <c r="AH242">
+        <v>1.43</v>
+      </c>
+      <c r="AI242">
+        <v>3.46</v>
+      </c>
+      <c r="AJ242">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>6</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C243" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D243" s="2">
+        <v>45320</v>
+      </c>
+      <c r="E243" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F243" t="s">
+        <v>201</v>
+      </c>
+      <c r="G243" t="s">
+        <v>40</v>
+      </c>
+      <c r="H243" t="s">
+        <v>41</v>
+      </c>
+      <c r="I243">
+        <v>3</v>
+      </c>
+      <c r="J243" t="s">
+        <v>204</v>
+      </c>
+      <c r="K243" t="s">
+        <v>144</v>
+      </c>
+      <c r="L243">
+        <v>99</v>
+      </c>
+      <c r="M243">
+        <v>75</v>
+      </c>
+      <c r="N243">
+        <v>616</v>
+      </c>
+      <c r="O243">
+        <v>746</v>
+      </c>
+      <c r="P243">
+        <v>6</v>
+      </c>
+      <c r="Q243">
+        <v>4</v>
+      </c>
+      <c r="R243">
+        <v>7</v>
+      </c>
+      <c r="S243">
+        <v>6</v>
+      </c>
+      <c r="Z243">
+        <v>2</v>
+      </c>
+      <c r="AA243">
+        <v>0</v>
+      </c>
+      <c r="AB243" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC243">
+        <v>1.91</v>
+      </c>
+      <c r="AD243">
+        <v>1.91</v>
+      </c>
+      <c r="AE243">
+        <v>1.94</v>
+      </c>
+      <c r="AF243">
+        <v>1.94</v>
+      </c>
+      <c r="AG243">
+        <v>1.95</v>
+      </c>
+      <c r="AH243">
+        <v>2</v>
+      </c>
+      <c r="AI243">
+        <v>1.88</v>
+      </c>
+      <c r="AJ243">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="244" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>6</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D244" s="2">
+        <v>45321</v>
+      </c>
+      <c r="E244" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F244" t="s">
+        <v>201</v>
+      </c>
+      <c r="G244" t="s">
+        <v>40</v>
+      </c>
+      <c r="H244" t="s">
+        <v>41</v>
+      </c>
+      <c r="I244">
+        <v>3</v>
+      </c>
+      <c r="J244" t="s">
+        <v>133</v>
+      </c>
+      <c r="K244" t="s">
+        <v>205</v>
+      </c>
+      <c r="L244">
+        <v>71</v>
+      </c>
+      <c r="M244">
+        <v>172</v>
+      </c>
+      <c r="N244">
+        <v>768</v>
+      </c>
+      <c r="O244">
+        <v>354</v>
+      </c>
+      <c r="P244">
+        <v>7</v>
+      </c>
+      <c r="Q244">
+        <v>6</v>
+      </c>
+      <c r="R244">
+        <v>6</v>
+      </c>
+      <c r="S244">
+        <v>3</v>
+      </c>
+      <c r="Z244">
+        <v>2</v>
+      </c>
+      <c r="AA244">
+        <v>0</v>
+      </c>
+      <c r="AB244" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC244">
+        <v>1.44</v>
+      </c>
+      <c r="AD244">
+        <v>2.75</v>
+      </c>
+      <c r="AE244">
+        <v>1.49</v>
+      </c>
+      <c r="AF244">
+        <v>2.79</v>
+      </c>
+      <c r="AG244">
+        <v>1.49</v>
+      </c>
+      <c r="AH244">
+        <v>2.8</v>
+      </c>
+      <c r="AI244">
+        <v>1.45</v>
+      </c>
+      <c r="AJ244">
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="245" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>6</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C245" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D245" s="2">
+        <v>45321</v>
+      </c>
+      <c r="E245" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F245" t="s">
+        <v>201</v>
+      </c>
+      <c r="G245" t="s">
+        <v>40</v>
+      </c>
+      <c r="H245" t="s">
+        <v>41</v>
+      </c>
+      <c r="I245">
+        <v>3</v>
+      </c>
+      <c r="J245" t="s">
+        <v>193</v>
+      </c>
+      <c r="K245" t="s">
+        <v>206</v>
+      </c>
+      <c r="L245">
+        <v>104</v>
+      </c>
+      <c r="M245">
+        <v>214</v>
+      </c>
+      <c r="N245">
+        <v>591</v>
+      </c>
+      <c r="O245">
+        <v>287</v>
+      </c>
+      <c r="P245">
+        <v>6</v>
+      </c>
+      <c r="Q245">
+        <v>7</v>
+      </c>
+      <c r="R245">
+        <v>6</v>
+      </c>
+      <c r="S245">
+        <v>4</v>
+      </c>
+      <c r="T245">
+        <v>6</v>
+      </c>
+      <c r="U245">
+        <v>2</v>
+      </c>
+      <c r="Z245">
+        <v>2</v>
+      </c>
+      <c r="AA245">
+        <v>1</v>
+      </c>
+      <c r="AB245" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC245">
+        <v>1.53</v>
+      </c>
+      <c r="AD245">
+        <v>2.5</v>
+      </c>
+      <c r="AE245">
+        <v>1.63</v>
+      </c>
+      <c r="AF245">
+        <v>2.41</v>
+      </c>
+      <c r="AG245">
+        <v>1.63</v>
+      </c>
+      <c r="AH245">
+        <v>2.88</v>
+      </c>
+      <c r="AI245">
+        <v>1.55</v>
+      </c>
+      <c r="AJ245">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="246" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>6</v>
+      </c>
+      <c r="B246" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C246" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D246" s="2">
+        <v>45321</v>
+      </c>
+      <c r="E246" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F246" t="s">
+        <v>201</v>
+      </c>
+      <c r="G246" t="s">
+        <v>40</v>
+      </c>
+      <c r="H246" t="s">
+        <v>41</v>
+      </c>
+      <c r="I246">
+        <v>3</v>
+      </c>
+      <c r="J246" t="s">
+        <v>207</v>
+      </c>
+      <c r="K246" t="s">
+        <v>208</v>
+      </c>
+      <c r="L246">
+        <v>144</v>
+      </c>
+      <c r="M246">
+        <v>315</v>
+      </c>
+      <c r="N246">
+        <v>449</v>
+      </c>
+      <c r="O246">
+        <v>172</v>
+      </c>
+      <c r="P246">
+        <v>6</v>
+      </c>
+      <c r="Q246">
+        <v>4</v>
+      </c>
+      <c r="R246">
+        <v>7</v>
+      </c>
+      <c r="S246">
+        <v>5</v>
+      </c>
+      <c r="Z246">
+        <v>2</v>
+      </c>
+      <c r="AA246">
+        <v>0</v>
+      </c>
+      <c r="AB246" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC246">
+        <v>1.91</v>
+      </c>
+      <c r="AD246">
+        <v>1.91</v>
+      </c>
+      <c r="AE246">
+        <v>1.99</v>
+      </c>
+      <c r="AF246">
+        <v>1.89</v>
+      </c>
+      <c r="AG246">
+        <v>1.99</v>
+      </c>
+      <c r="AH246">
+        <v>2.1</v>
+      </c>
+      <c r="AI246">
+        <v>1.89</v>
+      </c>
+      <c r="AJ246">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="247" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>6</v>
+      </c>
+      <c r="B247" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C247" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D247" s="2">
+        <v>45321</v>
+      </c>
+      <c r="E247" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F247" t="s">
+        <v>201</v>
+      </c>
+      <c r="G247" t="s">
+        <v>40</v>
+      </c>
+      <c r="H247" t="s">
+        <v>41</v>
+      </c>
+      <c r="I247">
+        <v>3</v>
+      </c>
+      <c r="J247" t="s">
+        <v>136</v>
+      </c>
+      <c r="K247" t="s">
+        <v>160</v>
+      </c>
+      <c r="L247">
+        <v>137</v>
+      </c>
+      <c r="M247">
+        <v>88</v>
+      </c>
+      <c r="N247">
+        <v>480</v>
+      </c>
+      <c r="O247">
+        <v>684</v>
+      </c>
+      <c r="P247">
+        <v>6</v>
+      </c>
+      <c r="Q247">
+        <v>1</v>
+      </c>
+      <c r="R247">
+        <v>6</v>
+      </c>
+      <c r="S247">
+        <v>3</v>
+      </c>
+      <c r="Z247">
+        <v>2</v>
+      </c>
+      <c r="AA247">
+        <v>0</v>
+      </c>
+      <c r="AB247" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC247">
+        <v>1.8</v>
+      </c>
+      <c r="AD247">
+        <v>2</v>
+      </c>
+      <c r="AE247">
+        <v>1.92</v>
+      </c>
+      <c r="AF247">
+        <v>1.97</v>
+      </c>
+      <c r="AG247">
+        <v>1.92</v>
+      </c>
+      <c r="AH247">
+        <v>2.12</v>
+      </c>
+      <c r="AI247">
+        <v>1.78</v>
+      </c>
+      <c r="AJ247">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="248" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>6</v>
+      </c>
+      <c r="B248" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C248" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D248" s="2">
+        <v>45321</v>
+      </c>
+      <c r="E248" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F248" t="s">
+        <v>201</v>
+      </c>
+      <c r="G248" t="s">
+        <v>40</v>
+      </c>
+      <c r="H248" t="s">
+        <v>41</v>
+      </c>
+      <c r="I248">
+        <v>3</v>
+      </c>
+      <c r="J248" t="s">
+        <v>183</v>
+      </c>
+      <c r="K248" t="s">
+        <v>175</v>
+      </c>
+      <c r="L248">
+        <v>83</v>
+      </c>
+      <c r="M248">
+        <v>92</v>
+      </c>
+      <c r="N248">
+        <v>696</v>
+      </c>
+      <c r="O248">
+        <v>636</v>
+      </c>
+      <c r="P248">
+        <v>6</v>
+      </c>
+      <c r="Q248">
+        <v>1</v>
+      </c>
+      <c r="R248">
+        <v>6</v>
+      </c>
+      <c r="S248">
+        <v>3</v>
+      </c>
+      <c r="Z248">
+        <v>2</v>
+      </c>
+      <c r="AA248">
+        <v>0</v>
+      </c>
+      <c r="AB248" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC248">
+        <v>1.4</v>
+      </c>
+      <c r="AD248">
+        <v>3</v>
+      </c>
+      <c r="AE248">
+        <v>1.4</v>
+      </c>
+      <c r="AF248">
+        <v>3.18</v>
+      </c>
+      <c r="AG248">
+        <v>1.41</v>
+      </c>
+      <c r="AH248">
+        <v>3.2</v>
+      </c>
+      <c r="AI248">
+        <v>1.38</v>
+      </c>
+      <c r="AJ248">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="249" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>6</v>
+      </c>
+      <c r="B249" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C249" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D249" s="2">
+        <v>45321</v>
+      </c>
+      <c r="E249" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F249" t="s">
+        <v>201</v>
+      </c>
+      <c r="G249" t="s">
+        <v>40</v>
+      </c>
+      <c r="H249" t="s">
+        <v>41</v>
+      </c>
+      <c r="I249">
+        <v>3</v>
+      </c>
+      <c r="J249" t="s">
+        <v>209</v>
+      </c>
+      <c r="K249" t="s">
+        <v>138</v>
+      </c>
+      <c r="L249">
+        <v>156</v>
+      </c>
+      <c r="M249">
+        <v>130</v>
+      </c>
+      <c r="N249">
+        <v>404</v>
+      </c>
+      <c r="O249">
+        <v>500</v>
+      </c>
+      <c r="P249">
+        <v>7</v>
+      </c>
+      <c r="Q249">
+        <v>6</v>
+      </c>
+      <c r="R249">
+        <v>7</v>
+      </c>
+      <c r="S249">
+        <v>5</v>
+      </c>
+      <c r="Z249">
+        <v>2</v>
+      </c>
+      <c r="AA249">
+        <v>0</v>
+      </c>
+      <c r="AB249" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC249">
+        <v>2.63</v>
+      </c>
+      <c r="AD249">
+        <v>1.5</v>
+      </c>
+      <c r="AE249">
+        <v>2.44</v>
+      </c>
+      <c r="AF249">
+        <v>1.61</v>
+      </c>
+      <c r="AG249">
+        <v>2.95</v>
+      </c>
+      <c r="AH249">
+        <v>1.61</v>
+      </c>
+      <c r="AI249">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="AJ249">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="250" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>6</v>
+      </c>
+      <c r="B250" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C250" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D250" s="2">
+        <v>45322</v>
+      </c>
+      <c r="E250" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F250" t="s">
+        <v>201</v>
+      </c>
+      <c r="G250" t="s">
+        <v>40</v>
+      </c>
+      <c r="H250" t="s">
+        <v>41</v>
+      </c>
+      <c r="I250">
+        <v>3</v>
+      </c>
+      <c r="J250" t="s">
+        <v>45</v>
+      </c>
+      <c r="K250" t="s">
+        <v>210</v>
+      </c>
+      <c r="L250">
+        <v>59</v>
+      </c>
+      <c r="M250">
+        <v>194</v>
+      </c>
+      <c r="N250">
+        <v>885</v>
+      </c>
+      <c r="O250">
+        <v>315</v>
+      </c>
+      <c r="P250">
+        <v>6</v>
+      </c>
+      <c r="Q250">
+        <v>4</v>
+      </c>
+      <c r="R250">
+        <v>4</v>
+      </c>
+      <c r="S250">
+        <v>6</v>
+      </c>
+      <c r="T250">
+        <v>6</v>
+      </c>
+      <c r="U250">
+        <v>4</v>
+      </c>
+      <c r="Z250">
+        <v>2</v>
+      </c>
+      <c r="AA250">
+        <v>1</v>
+      </c>
+      <c r="AB250" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC250">
+        <v>1.36</v>
+      </c>
+      <c r="AD250">
+        <v>3.2</v>
+      </c>
+      <c r="AE250">
+        <v>1.43</v>
+      </c>
+      <c r="AF250">
+        <v>3.02</v>
+      </c>
+      <c r="AG250">
+        <v>1.43</v>
+      </c>
+      <c r="AH250">
+        <v>3.25</v>
+      </c>
+      <c r="AI250">
+        <v>1.36</v>
+      </c>
+      <c r="AJ250">
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="251" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>6</v>
+      </c>
+      <c r="B251" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C251" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D251" s="2">
+        <v>45322</v>
+      </c>
+      <c r="E251" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F251" t="s">
+        <v>201</v>
+      </c>
+      <c r="G251" t="s">
+        <v>40</v>
+      </c>
+      <c r="H251" t="s">
+        <v>41</v>
+      </c>
+      <c r="I251">
+        <v>3</v>
+      </c>
+      <c r="J251" t="s">
+        <v>164</v>
+      </c>
+      <c r="K251" t="s">
+        <v>115</v>
+      </c>
+      <c r="L251">
+        <v>106</v>
+      </c>
+      <c r="M251">
+        <v>80</v>
+      </c>
+      <c r="N251">
+        <v>584</v>
+      </c>
+      <c r="O251">
+        <v>715</v>
+      </c>
+      <c r="P251">
+        <v>4</v>
+      </c>
+      <c r="Q251">
+        <v>6</v>
+      </c>
+      <c r="R251">
+        <v>6</v>
+      </c>
+      <c r="S251">
+        <v>4</v>
+      </c>
+      <c r="T251">
+        <v>6</v>
+      </c>
+      <c r="U251">
+        <v>2</v>
+      </c>
+      <c r="Z251">
+        <v>2</v>
+      </c>
+      <c r="AA251">
+        <v>1</v>
+      </c>
+      <c r="AB251" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC251">
+        <v>1.25</v>
+      </c>
+      <c r="AD251">
+        <v>4</v>
+      </c>
+      <c r="AE251">
+        <v>1.33</v>
+      </c>
+      <c r="AF251">
+        <v>3.6</v>
+      </c>
+      <c r="AG251">
+        <v>1.33</v>
+      </c>
+      <c r="AH251">
+        <v>4.05</v>
+      </c>
+      <c r="AI251">
+        <v>1.25</v>
+      </c>
+      <c r="AJ251">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="252" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>6</v>
+      </c>
+      <c r="B252" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C252" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D252" s="2">
+        <v>45322</v>
+      </c>
+      <c r="E252" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F252" t="s">
+        <v>201</v>
+      </c>
+      <c r="G252" t="s">
+        <v>40</v>
+      </c>
+      <c r="H252" t="s">
+        <v>41</v>
+      </c>
+      <c r="I252">
+        <v>3</v>
+      </c>
+      <c r="J252" t="s">
+        <v>159</v>
+      </c>
+      <c r="K252" t="s">
+        <v>134</v>
+      </c>
+      <c r="L252">
+        <v>76</v>
+      </c>
+      <c r="M252">
+        <v>70</v>
+      </c>
+      <c r="N252">
+        <v>738</v>
+      </c>
+      <c r="O252">
+        <v>787</v>
+      </c>
+      <c r="P252">
+        <v>6</v>
+      </c>
+      <c r="Q252">
+        <v>7</v>
+      </c>
+      <c r="R252">
+        <v>6</v>
+      </c>
+      <c r="S252">
+        <v>3</v>
+      </c>
+      <c r="T252">
+        <v>6</v>
+      </c>
+      <c r="U252">
+        <v>0</v>
+      </c>
+      <c r="Z252">
+        <v>2</v>
+      </c>
+      <c r="AA252">
+        <v>1</v>
+      </c>
+      <c r="AB252" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC252">
+        <v>3.4</v>
+      </c>
+      <c r="AD252">
+        <v>1.33</v>
+      </c>
+      <c r="AE252">
+        <v>3.6</v>
+      </c>
+      <c r="AF252">
+        <v>1.33</v>
+      </c>
+      <c r="AG252">
+        <v>3.6</v>
+      </c>
+      <c r="AH252">
+        <v>1.35</v>
+      </c>
+      <c r="AI252">
+        <v>3.29</v>
+      </c>
+      <c r="AJ252">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="253" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>6</v>
+      </c>
+      <c r="B253" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C253" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D253" s="2">
+        <v>45322</v>
+      </c>
+      <c r="E253" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F253" t="s">
+        <v>201</v>
+      </c>
+      <c r="G253" t="s">
+        <v>40</v>
+      </c>
+      <c r="H253" t="s">
+        <v>76</v>
+      </c>
+      <c r="I253">
+        <v>3</v>
+      </c>
+      <c r="J253" t="s">
+        <v>202</v>
+      </c>
+      <c r="K253" t="s">
+        <v>133</v>
+      </c>
+      <c r="L253">
+        <v>133</v>
+      </c>
+      <c r="M253">
+        <v>71</v>
+      </c>
+      <c r="N253">
+        <v>497</v>
+      </c>
+      <c r="O253">
+        <v>768</v>
+      </c>
+      <c r="P253">
+        <v>6</v>
+      </c>
+      <c r="Q253">
+        <v>4</v>
+      </c>
+      <c r="R253">
+        <v>6</v>
+      </c>
+      <c r="S253">
+        <v>4</v>
+      </c>
+      <c r="Z253">
+        <v>2</v>
+      </c>
+      <c r="AA253">
+        <v>0</v>
+      </c>
+      <c r="AB253" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC253">
+        <v>2.1</v>
+      </c>
+      <c r="AD253">
+        <v>1.73</v>
+      </c>
+      <c r="AE253">
+        <v>2.19</v>
+      </c>
+      <c r="AF253">
+        <v>1.76</v>
+      </c>
+      <c r="AG253">
+        <v>2.19</v>
+      </c>
+      <c r="AH253">
+        <v>1.8</v>
+      </c>
+      <c r="AI253">
+        <v>2.04</v>
+      </c>
+      <c r="AJ253">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="254" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>6</v>
+      </c>
+      <c r="B254" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C254" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D254" s="2">
+        <v>45322</v>
+      </c>
+      <c r="E254" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F254" t="s">
+        <v>201</v>
+      </c>
+      <c r="G254" t="s">
+        <v>40</v>
+      </c>
+      <c r="H254" t="s">
+        <v>76</v>
+      </c>
+      <c r="I254">
+        <v>3</v>
+      </c>
+      <c r="J254" t="s">
+        <v>207</v>
+      </c>
+      <c r="K254" t="s">
+        <v>203</v>
+      </c>
+      <c r="L254">
+        <v>144</v>
+      </c>
+      <c r="M254">
+        <v>112</v>
+      </c>
+      <c r="N254">
+        <v>449</v>
+      </c>
+      <c r="O254">
+        <v>551</v>
+      </c>
+      <c r="P254">
+        <v>6</v>
+      </c>
+      <c r="Q254">
+        <v>1</v>
+      </c>
+      <c r="R254">
+        <v>6</v>
+      </c>
+      <c r="S254">
+        <v>4</v>
+      </c>
+      <c r="Z254">
+        <v>2</v>
+      </c>
+      <c r="AA254">
+        <v>0</v>
+      </c>
+      <c r="AB254" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC254">
+        <v>1.53</v>
+      </c>
+      <c r="AD254">
+        <v>2.5</v>
+      </c>
+      <c r="AE254">
+        <v>1.5</v>
+      </c>
+      <c r="AF254">
+        <v>2.78</v>
+      </c>
+      <c r="AG254">
+        <v>1.58</v>
+      </c>
+      <c r="AH254">
+        <v>2.78</v>
+      </c>
+      <c r="AI254">
+        <v>1.52</v>
+      </c>
+      <c r="AJ254">
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="255" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>6</v>
+      </c>
+      <c r="B255" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C255" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D255" s="2">
+        <v>45322</v>
+      </c>
+      <c r="E255" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F255" t="s">
+        <v>201</v>
+      </c>
+      <c r="G255" t="s">
+        <v>40</v>
+      </c>
+      <c r="H255" t="s">
+        <v>76</v>
+      </c>
+      <c r="I255">
+        <v>3</v>
+      </c>
+      <c r="J255" t="s">
+        <v>123</v>
+      </c>
+      <c r="K255" t="s">
+        <v>136</v>
+      </c>
+      <c r="L255">
+        <v>27</v>
+      </c>
+      <c r="M255">
+        <v>137</v>
+      </c>
+      <c r="N255">
+        <v>1459</v>
+      </c>
+      <c r="O255">
+        <v>480</v>
+      </c>
+      <c r="P255">
+        <v>1</v>
+      </c>
+      <c r="Q255">
+        <v>6</v>
+      </c>
+      <c r="R255">
+        <v>7</v>
+      </c>
+      <c r="S255">
+        <v>6</v>
+      </c>
+      <c r="T255">
+        <v>6</v>
+      </c>
+      <c r="U255">
+        <v>3</v>
+      </c>
+      <c r="Z255">
+        <v>2</v>
+      </c>
+      <c r="AA255">
+        <v>1</v>
+      </c>
+      <c r="AB255" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC255">
+        <v>1.73</v>
+      </c>
+      <c r="AD255">
+        <v>2.1</v>
+      </c>
+      <c r="AE255">
+        <v>1.8</v>
+      </c>
+      <c r="AF255">
+        <v>2.13</v>
+      </c>
+      <c r="AG255">
+        <v>1.8</v>
+      </c>
+      <c r="AH255">
+        <v>2.13</v>
+      </c>
+      <c r="AI255">
+        <v>1.76</v>
+      </c>
+      <c r="AJ255">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="256" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>6</v>
+      </c>
+      <c r="B256" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C256" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D256" s="2">
+        <v>45323</v>
+      </c>
+      <c r="E256" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F256" t="s">
+        <v>201</v>
+      </c>
+      <c r="G256" t="s">
+        <v>40</v>
+      </c>
+      <c r="H256" t="s">
+        <v>76</v>
+      </c>
+      <c r="I256">
+        <v>3</v>
+      </c>
+      <c r="J256" t="s">
+        <v>45</v>
+      </c>
+      <c r="K256" t="s">
+        <v>193</v>
+      </c>
+      <c r="L256">
+        <v>59</v>
+      </c>
+      <c r="M256">
+        <v>104</v>
+      </c>
+      <c r="N256">
+        <v>885</v>
+      </c>
+      <c r="O256">
+        <v>591</v>
+      </c>
+      <c r="P256">
+        <v>7</v>
+      </c>
+      <c r="Q256">
+        <v>6</v>
+      </c>
+      <c r="R256">
+        <v>2</v>
+      </c>
+      <c r="S256">
+        <v>6</v>
+      </c>
+      <c r="T256">
+        <v>6</v>
+      </c>
+      <c r="U256">
+        <v>3</v>
+      </c>
+      <c r="Z256">
+        <v>2</v>
+      </c>
+      <c r="AA256">
+        <v>1</v>
+      </c>
+      <c r="AB256" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC256">
+        <v>1.8</v>
+      </c>
+      <c r="AD256">
+        <v>2</v>
+      </c>
+      <c r="AE256">
+        <v>1.93</v>
+      </c>
+      <c r="AF256">
+        <v>1.98</v>
+      </c>
+      <c r="AG256">
+        <v>1.93</v>
+      </c>
+      <c r="AH256">
+        <v>2.14</v>
+      </c>
+      <c r="AI256">
+        <v>1.83</v>
+      </c>
+      <c r="AJ256">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="257" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>6</v>
+      </c>
+      <c r="B257" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C257" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D257" s="2">
+        <v>45323</v>
+      </c>
+      <c r="E257" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F257" t="s">
+        <v>201</v>
+      </c>
+      <c r="G257" t="s">
+        <v>40</v>
+      </c>
+      <c r="H257" t="s">
+        <v>76</v>
+      </c>
+      <c r="I257">
+        <v>3</v>
+      </c>
+      <c r="J257" t="s">
+        <v>156</v>
+      </c>
+      <c r="K257" t="s">
+        <v>204</v>
+      </c>
+      <c r="L257">
+        <v>37</v>
+      </c>
+      <c r="M257">
+        <v>99</v>
+      </c>
+      <c r="N257">
+        <v>1154</v>
+      </c>
+      <c r="O257">
+        <v>616</v>
+      </c>
+      <c r="P257">
+        <v>6</v>
+      </c>
+      <c r="Q257">
+        <v>4</v>
+      </c>
+      <c r="R257">
+        <v>6</v>
+      </c>
+      <c r="S257">
+        <v>0</v>
+      </c>
+      <c r="Z257">
+        <v>2</v>
+      </c>
+      <c r="AA257">
+        <v>0</v>
+      </c>
+      <c r="AB257" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC257">
+        <v>1.36</v>
+      </c>
+      <c r="AD257">
+        <v>3.2</v>
+      </c>
+      <c r="AE257">
+        <v>1.43</v>
+      </c>
+      <c r="AF257">
+        <v>3.07</v>
+      </c>
+      <c r="AG257">
+        <v>1.43</v>
+      </c>
+      <c r="AH257">
+        <v>3.2</v>
+      </c>
+      <c r="AI257">
+        <v>1.37</v>
+      </c>
+      <c r="AJ257">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="258" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>6</v>
+      </c>
+      <c r="B258" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C258" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D258" s="2">
+        <v>45323</v>
+      </c>
+      <c r="E258" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F258" t="s">
+        <v>201</v>
+      </c>
+      <c r="G258" t="s">
+        <v>40</v>
+      </c>
+      <c r="H258" t="s">
+        <v>76</v>
+      </c>
+      <c r="I258">
+        <v>3</v>
+      </c>
+      <c r="J258" t="s">
+        <v>159</v>
+      </c>
+      <c r="K258" t="s">
+        <v>164</v>
+      </c>
+      <c r="L258">
+        <v>76</v>
+      </c>
+      <c r="M258">
+        <v>106</v>
+      </c>
+      <c r="N258">
+        <v>738</v>
+      </c>
+      <c r="O258">
+        <v>584</v>
+      </c>
+      <c r="P258">
+        <v>6</v>
+      </c>
+      <c r="Q258">
+        <v>4</v>
+      </c>
+      <c r="R258">
+        <v>6</v>
+      </c>
+      <c r="S258">
+        <v>1</v>
+      </c>
+      <c r="Z258">
+        <v>2</v>
+      </c>
+      <c r="AA258">
+        <v>0</v>
+      </c>
+      <c r="AB258" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC258">
+        <v>1.53</v>
+      </c>
+      <c r="AD258">
+        <v>2.5</v>
+      </c>
+      <c r="AE258">
+        <v>1.69</v>
+      </c>
+      <c r="AF258">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AG258">
+        <v>1.69</v>
+      </c>
+      <c r="AH258">
+        <v>2.67</v>
+      </c>
+      <c r="AI258">
+        <v>1.56</v>
+      </c>
+      <c r="AJ258">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="259" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>6</v>
+      </c>
+      <c r="B259" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C259" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D259" s="2">
+        <v>45323</v>
+      </c>
+      <c r="E259" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F259" t="s">
+        <v>201</v>
+      </c>
+      <c r="G259" t="s">
+        <v>40</v>
+      </c>
+      <c r="H259" t="s">
+        <v>76</v>
+      </c>
+      <c r="I259">
+        <v>3</v>
+      </c>
+      <c r="J259" t="s">
+        <v>139</v>
+      </c>
+      <c r="K259" t="s">
+        <v>183</v>
+      </c>
+      <c r="L259">
+        <v>30</v>
+      </c>
+      <c r="M259">
+        <v>83</v>
+      </c>
+      <c r="N259">
+        <v>1345</v>
+      </c>
+      <c r="O259">
+        <v>696</v>
+      </c>
+      <c r="P259">
+        <v>7</v>
+      </c>
+      <c r="Q259">
+        <v>5</v>
+      </c>
+      <c r="R259">
+        <v>2</v>
+      </c>
+      <c r="S259">
+        <v>6</v>
+      </c>
+      <c r="T259">
+        <v>7</v>
+      </c>
+      <c r="U259">
+        <v>6</v>
+      </c>
+      <c r="Z259">
+        <v>2</v>
+      </c>
+      <c r="AA259">
+        <v>1</v>
+      </c>
+      <c r="AB259" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC259">
+        <v>2</v>
+      </c>
+      <c r="AD259">
+        <v>1.8</v>
+      </c>
+      <c r="AE259">
+        <v>2.1</v>
+      </c>
+      <c r="AF259">
+        <v>1.83</v>
+      </c>
+      <c r="AG259">
+        <v>2.1</v>
+      </c>
+      <c r="AH259">
+        <v>1.83</v>
+      </c>
+      <c r="AI259">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AJ259">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="260" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>6</v>
+      </c>
+      <c r="B260" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C260" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D260" s="2">
+        <v>45323</v>
+      </c>
+      <c r="E260" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F260" t="s">
+        <v>201</v>
+      </c>
+      <c r="G260" t="s">
+        <v>40</v>
+      </c>
+      <c r="H260" t="s">
+        <v>76</v>
+      </c>
+      <c r="I260">
+        <v>3</v>
+      </c>
+      <c r="J260" t="s">
+        <v>49</v>
+      </c>
+      <c r="K260" t="s">
+        <v>209</v>
+      </c>
+      <c r="L260">
+        <v>7</v>
+      </c>
+      <c r="M260">
+        <v>156</v>
+      </c>
+      <c r="N260">
+        <v>3685</v>
+      </c>
+      <c r="O260">
+        <v>404</v>
+      </c>
+      <c r="P260">
+        <v>7</v>
+      </c>
+      <c r="Q260">
+        <v>5</v>
+      </c>
+      <c r="R260">
+        <v>6</v>
+      </c>
+      <c r="S260">
+        <v>2</v>
+      </c>
+      <c r="Z260">
+        <v>2</v>
+      </c>
+      <c r="AA260">
+        <v>0</v>
+      </c>
+      <c r="AB260" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC260">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AD260">
+        <v>5.5</v>
+      </c>
+      <c r="AE260">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AF260">
+        <v>6.15</v>
+      </c>
+      <c r="AG260">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AH260">
+        <v>6.25</v>
+      </c>
+      <c r="AI260">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="AJ260">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="261" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>6</v>
+      </c>
+      <c r="B261" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C261" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D261" s="2">
+        <v>45324</v>
+      </c>
+      <c r="E261" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F261" t="s">
+        <v>201</v>
+      </c>
+      <c r="G261" t="s">
+        <v>40</v>
+      </c>
+      <c r="H261" t="s">
+        <v>78</v>
+      </c>
+      <c r="I261">
+        <v>3</v>
+      </c>
+      <c r="J261" t="s">
+        <v>123</v>
+      </c>
+      <c r="K261" t="s">
+        <v>45</v>
+      </c>
+      <c r="L261">
+        <v>27</v>
+      </c>
+      <c r="M261">
+        <v>59</v>
+      </c>
+      <c r="N261">
+        <v>1459</v>
+      </c>
+      <c r="O261">
+        <v>885</v>
+      </c>
+      <c r="P261">
+        <v>4</v>
+      </c>
+      <c r="Q261">
+        <v>6</v>
+      </c>
+      <c r="R261">
+        <v>6</v>
+      </c>
+      <c r="S261">
+        <v>3</v>
+      </c>
+      <c r="T261">
+        <v>6</v>
+      </c>
+      <c r="U261">
+        <v>4</v>
+      </c>
+      <c r="Z261">
+        <v>2</v>
+      </c>
+      <c r="AA261">
+        <v>1</v>
+      </c>
+      <c r="AB261" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC261">
+        <v>1.5</v>
+      </c>
+      <c r="AD261">
+        <v>2.63</v>
+      </c>
+      <c r="AE261">
+        <v>1.52</v>
+      </c>
+      <c r="AF261">
+        <v>2.72</v>
+      </c>
+      <c r="AG261">
+        <v>1.52</v>
+      </c>
+      <c r="AH261">
+        <v>2.75</v>
+      </c>
+      <c r="AI261">
+        <v>1.48</v>
+      </c>
+      <c r="AJ261">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="262" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>6</v>
+      </c>
+      <c r="B262" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C262" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D262" s="2">
+        <v>45324</v>
+      </c>
+      <c r="E262" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F262" t="s">
+        <v>201</v>
+      </c>
+      <c r="G262" t="s">
+        <v>40</v>
+      </c>
+      <c r="H262" t="s">
+        <v>78</v>
+      </c>
+      <c r="I262">
+        <v>3</v>
+      </c>
+      <c r="J262" t="s">
+        <v>139</v>
+      </c>
+      <c r="K262" t="s">
+        <v>207</v>
+      </c>
+      <c r="L262">
+        <v>30</v>
+      </c>
+      <c r="M262">
+        <v>144</v>
+      </c>
+      <c r="N262">
+        <v>1345</v>
+      </c>
+      <c r="O262">
+        <v>449</v>
+      </c>
+      <c r="P262">
+        <v>7</v>
+      </c>
+      <c r="Q262">
+        <v>5</v>
+      </c>
+      <c r="R262">
+        <v>6</v>
+      </c>
+      <c r="S262">
+        <v>1</v>
+      </c>
+      <c r="Z262">
+        <v>2</v>
+      </c>
+      <c r="AA262">
+        <v>0</v>
+      </c>
+      <c r="AB262" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC262">
+        <v>1.29</v>
+      </c>
+      <c r="AD262">
+        <v>3.75</v>
+      </c>
+      <c r="AE262">
+        <v>1.26</v>
+      </c>
+      <c r="AF262">
+        <v>4.29</v>
+      </c>
+      <c r="AG262">
+        <v>1.32</v>
+      </c>
+      <c r="AH262">
+        <v>4.29</v>
+      </c>
+      <c r="AI262">
+        <v>1.25</v>
+      </c>
+      <c r="AJ262">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="263" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>6</v>
+      </c>
+      <c r="B263" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C263" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D263" s="2">
+        <v>45324</v>
+      </c>
+      <c r="E263" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F263" t="s">
+        <v>201</v>
+      </c>
+      <c r="G263" t="s">
+        <v>40</v>
+      </c>
+      <c r="H263" t="s">
+        <v>78</v>
+      </c>
+      <c r="I263">
+        <v>3</v>
+      </c>
+      <c r="J263" t="s">
+        <v>49</v>
+      </c>
+      <c r="K263" t="s">
+        <v>202</v>
+      </c>
+      <c r="L263">
+        <v>7</v>
+      </c>
+      <c r="M263">
+        <v>133</v>
+      </c>
+      <c r="N263">
+        <v>3685</v>
+      </c>
+      <c r="O263">
+        <v>497</v>
+      </c>
+      <c r="P263">
+        <v>7</v>
+      </c>
+      <c r="Q263">
+        <v>6</v>
+      </c>
+      <c r="R263">
+        <v>6</v>
+      </c>
+      <c r="S263">
+        <v>4</v>
+      </c>
+      <c r="Z263">
+        <v>2</v>
+      </c>
+      <c r="AA263">
+        <v>0</v>
+      </c>
+      <c r="AB263" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC263">
+        <v>1.2</v>
+      </c>
+      <c r="AD263">
+        <v>4.5</v>
+      </c>
+      <c r="AE263">
+        <v>1.24</v>
+      </c>
+      <c r="AF263">
+        <v>4.59</v>
+      </c>
+      <c r="AG263">
+        <v>1.24</v>
+      </c>
+      <c r="AH263">
+        <v>5.24</v>
+      </c>
+      <c r="AI263">
+        <v>1.2</v>
+      </c>
+      <c r="AJ263">
+        <v>4.38</v>
+      </c>
+    </row>
+    <row r="264" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>6</v>
+      </c>
+      <c r="B264" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C264" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D264" s="2">
+        <v>45324</v>
+      </c>
+      <c r="E264" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F264" t="s">
+        <v>201</v>
+      </c>
+      <c r="G264" t="s">
+        <v>40</v>
+      </c>
+      <c r="H264" t="s">
+        <v>78</v>
+      </c>
+      <c r="I264">
+        <v>3</v>
+      </c>
+      <c r="J264" t="s">
+        <v>156</v>
+      </c>
+      <c r="K264" t="s">
+        <v>159</v>
+      </c>
+      <c r="L264">
+        <v>37</v>
+      </c>
+      <c r="M264">
+        <v>76</v>
+      </c>
+      <c r="N264">
+        <v>1154</v>
+      </c>
+      <c r="O264">
+        <v>738</v>
+      </c>
+      <c r="P264">
+        <v>6</v>
+      </c>
+      <c r="Q264">
+        <v>3</v>
+      </c>
+      <c r="R264">
+        <v>6</v>
+      </c>
+      <c r="S264">
+        <v>4</v>
+      </c>
+      <c r="Z264">
+        <v>2</v>
+      </c>
+      <c r="AA264">
+        <v>0</v>
+      </c>
+      <c r="AB264" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC264">
+        <v>1.44</v>
+      </c>
+      <c r="AD264">
+        <v>2.75</v>
+      </c>
+      <c r="AE264">
+        <v>1.49</v>
+      </c>
+      <c r="AF264">
+        <v>2.85</v>
+      </c>
+      <c r="AG264">
+        <v>1.52</v>
+      </c>
+      <c r="AH264">
+        <v>2.85</v>
+      </c>
+      <c r="AI264">
+        <v>1.46</v>
+      </c>
+      <c r="AJ264">
+        <v>2.66</v>
+      </c>
+    </row>
+    <row r="265" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>6</v>
+      </c>
+      <c r="B265" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C265" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D265" s="2">
+        <v>45325</v>
+      </c>
+      <c r="E265" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F265" t="s">
+        <v>201</v>
+      </c>
+      <c r="G265" t="s">
+        <v>40</v>
+      </c>
+      <c r="H265" t="s">
+        <v>79</v>
+      </c>
+      <c r="I265">
+        <v>3</v>
+      </c>
+      <c r="J265" t="s">
+        <v>123</v>
+      </c>
+      <c r="K265" t="s">
+        <v>139</v>
+      </c>
+      <c r="L265">
+        <v>27</v>
+      </c>
+      <c r="M265">
+        <v>30</v>
+      </c>
+      <c r="N265">
+        <v>1459</v>
+      </c>
+      <c r="O265">
+        <v>1345</v>
+      </c>
+      <c r="P265">
+        <v>4</v>
+      </c>
+      <c r="Q265">
+        <v>6</v>
+      </c>
+      <c r="R265">
+        <v>6</v>
+      </c>
+      <c r="S265">
+        <v>4</v>
+      </c>
+      <c r="T265">
+        <v>6</v>
+      </c>
+      <c r="U265">
+        <v>4</v>
+      </c>
+      <c r="Z265">
+        <v>2</v>
+      </c>
+      <c r="AA265">
+        <v>1</v>
+      </c>
+      <c r="AB265" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC265">
+        <v>2.63</v>
+      </c>
+      <c r="AD265">
+        <v>1.5</v>
+      </c>
+      <c r="AE265">
+        <v>2.62</v>
+      </c>
+      <c r="AF265">
+        <v>1.56</v>
+      </c>
+      <c r="AG265">
+        <v>2.75</v>
+      </c>
+      <c r="AH265">
+        <v>1.56</v>
+      </c>
+      <c r="AI265">
+        <v>2.59</v>
+      </c>
+      <c r="AJ265">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="266" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>6</v>
+      </c>
+      <c r="B266" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C266" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D266" s="2">
+        <v>45325</v>
+      </c>
+      <c r="E266" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F266" t="s">
+        <v>201</v>
+      </c>
+      <c r="G266" t="s">
+        <v>40</v>
+      </c>
+      <c r="H266" t="s">
+        <v>79</v>
+      </c>
+      <c r="I266">
+        <v>3</v>
+      </c>
+      <c r="J266" t="s">
+        <v>156</v>
+      </c>
+      <c r="K266" t="s">
+        <v>49</v>
+      </c>
+      <c r="L266">
+        <v>37</v>
+      </c>
+      <c r="M266">
+        <v>7</v>
+      </c>
+      <c r="N266">
+        <v>1154</v>
+      </c>
+      <c r="O266">
+        <v>3685</v>
+      </c>
+      <c r="P266">
+        <v>6</v>
+      </c>
+      <c r="Q266">
+        <v>3</v>
+      </c>
+      <c r="R266">
+        <v>4</v>
+      </c>
+      <c r="S266">
+        <v>1</v>
+      </c>
+      <c r="Z266">
+        <v>1</v>
+      </c>
+      <c r="AA266">
+        <v>0</v>
+      </c>
+      <c r="AB266" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC266">
+        <v>2.75</v>
+      </c>
+      <c r="AD266">
+        <v>1.44</v>
+      </c>
+      <c r="AE266">
+        <v>2.75</v>
+      </c>
+      <c r="AF266">
+        <v>1.52</v>
+      </c>
+      <c r="AG266">
+        <v>2.86</v>
+      </c>
+      <c r="AH266">
+        <v>1.52</v>
+      </c>
+      <c r="AI266">
+        <v>2.71</v>
+      </c>
+      <c r="AJ266">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="267" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>6</v>
+      </c>
+      <c r="B267" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C267" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D267" s="2">
+        <v>45326</v>
+      </c>
+      <c r="E267" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F267" t="s">
+        <v>201</v>
+      </c>
+      <c r="G267" t="s">
+        <v>40</v>
+      </c>
+      <c r="H267" t="s">
+        <v>80</v>
+      </c>
+      <c r="I267">
+        <v>3</v>
+      </c>
+      <c r="J267" t="s">
+        <v>123</v>
+      </c>
+      <c r="K267" t="s">
+        <v>156</v>
+      </c>
+      <c r="L267">
+        <v>27</v>
+      </c>
+      <c r="M267">
+        <v>37</v>
+      </c>
+      <c r="N267">
+        <v>1459</v>
+      </c>
+      <c r="O267">
+        <v>1154</v>
+      </c>
+      <c r="P267">
+        <v>5</v>
+      </c>
+      <c r="Q267">
+        <v>7</v>
+      </c>
+      <c r="R267">
+        <v>6</v>
+      </c>
+      <c r="S267">
+        <v>2</v>
+      </c>
+      <c r="T267">
+        <v>6</v>
+      </c>
+      <c r="U267">
+        <v>3</v>
+      </c>
+      <c r="Z267">
+        <v>2</v>
+      </c>
+      <c r="AA267">
+        <v>1</v>
+      </c>
+      <c r="AB267" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC267">
+        <v>2</v>
+      </c>
+      <c r="AD267">
+        <v>1.8</v>
+      </c>
+      <c r="AE267">
+        <v>2.06</v>
+      </c>
+      <c r="AF267">
+        <v>1.85</v>
+      </c>
+      <c r="AG267">
+        <v>2.06</v>
+      </c>
+      <c r="AH267">
+        <v>1.91</v>
+      </c>
+      <c r="AI267">
+        <v>1.98</v>
+      </c>
+      <c r="AJ267">
+        <v>1.81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>